<commit_message>
change values in database
</commit_message>
<xml_diff>
--- a/Work/Data/nf_db.xlsx
+++ b/Work/Data/nf_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veetalya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veetalya\Desktop\python-project-1\Work\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A96DB47-5B11-4A51-98E9-FC62ADFBEE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A95249-027F-4FA2-BCAA-3FB282B9A231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5124" yWindow="1980" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 нф" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +572,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="5">
-        <v>1232</v>
+        <v>1200</v>
       </c>
       <c r="J3" s="4">
         <v>1232</v>
@@ -601,7 +601,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="5">
-        <v>1232</v>
+        <v>1270</v>
       </c>
       <c r="J4" s="4">
         <v>1230</v>
@@ -630,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="5">
-        <v>1232</v>
+        <v>1176</v>
       </c>
       <c r="J5" s="4">
         <v>1235</v>
@@ -688,7 +688,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="5">
-        <v>11887</v>
+        <v>12503</v>
       </c>
       <c r="J7" s="4">
         <v>11887</v>
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="5">
-        <v>11887</v>
+        <v>11300</v>
       </c>
       <c r="J8" s="4">
         <v>11890</v>
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="5">
-        <v>11887</v>
+        <v>11670</v>
       </c>
       <c r="J9" s="4">
         <v>11892</v>

</xml_diff>